<commit_message>
Added Repustate Amazon Classification Report to Total
</commit_message>
<xml_diff>
--- a/Datasets/Calculation Result/Classification Report/Classification Report Total.xlsx
+++ b/Datasets/Calculation Result/Classification Report/Classification Report Total.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Calculation Result\Classification Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42720BEE-AD16-4E38-AAF2-437350DF7AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59CC268-20EC-4885-A814-F7EA53DA4031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7050" yWindow="2220" windowWidth="28110" windowHeight="16440" xr2:uid="{356F8004-839F-4170-968A-E905A86D7A5F}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="16200" xr2:uid="{356F8004-839F-4170-968A-E905A86D7A5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="104">
   <si>
     <t>Stanford</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>0.80</t>
+  </si>
+  <si>
+    <t>Repustate .5 Threshold</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +417,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -421,10 +428,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -741,86 +748,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7679C0-E6FB-4780-AA1A-EA6D9AA2FADC}">
-  <dimension ref="A1:AE96"/>
+  <dimension ref="A1:AM96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S16" workbookViewId="0">
-      <selection activeCell="AB47" sqref="AB47"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="9"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
       <c r="O1" s="2"/>
       <c r="Q1" s="12"/>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
       <c r="W1" s="12"/>
       <c r="Y1" s="14"/>
-      <c r="Z1" s="16" t="s">
+      <c r="Z1" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
       <c r="AE1" s="14"/>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="16"/>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
       <c r="G2" s="9"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
       <c r="O2" s="2"/>
       <c r="Q2" s="12"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
       <c r="W2" s="12"/>
       <c r="Y2" s="14"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
       <c r="AE2" s="14"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="16"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -832,15 +855,15 @@
       <c r="D3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="22" t="s">
         <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -852,14 +875,14 @@
       <c r="L3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="20"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="R3" s="12" t="s">
@@ -871,14 +894,14 @@
       <c r="T3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="U3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="18"/>
+      <c r="V3" s="20"/>
       <c r="W3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Y3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="Z3" s="14" t="s">
@@ -890,16 +913,35 @@
       <c r="AB3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AC3" s="18" t="s">
+      <c r="AC3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="18"/>
+      <c r="AD3" s="20"/>
       <c r="AE3" s="15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="AG3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -909,15 +951,15 @@
       <c r="D4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="10">
         <v>504</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="19"/>
+      <c r="I4" s="22"/>
       <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
@@ -927,14 +969,14 @@
       <c r="L4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="20"/>
+      <c r="N4" s="21"/>
       <c r="O4" s="3">
         <v>504</v>
       </c>
-      <c r="Q4" s="16"/>
+      <c r="Q4" s="18"/>
       <c r="R4" s="12" t="s">
         <v>6</v>
       </c>
@@ -944,14 +986,14 @@
       <c r="T4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="U4" s="18" t="s">
+      <c r="U4" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="V4" s="18"/>
+      <c r="V4" s="20"/>
       <c r="W4" s="13">
         <v>504</v>
       </c>
-      <c r="Y4" s="16"/>
+      <c r="Y4" s="18"/>
       <c r="Z4" s="14" t="s">
         <v>6</v>
       </c>
@@ -961,16 +1003,33 @@
       <c r="AB4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="AC4" s="18" t="s">
+      <c r="AC4" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="AD4" s="18"/>
+      <c r="AD4" s="20"/>
       <c r="AE4" s="15">
         <v>504</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ4" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK4" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="17">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
@@ -980,15 +1039,15 @@
       <c r="D5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="10">
         <v>496</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="19"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="2" t="s">
         <v>7</v>
       </c>
@@ -998,14 +1057,14 @@
       <c r="L5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N5" s="20"/>
+      <c r="N5" s="21"/>
       <c r="O5" s="3">
         <v>496</v>
       </c>
-      <c r="Q5" s="16"/>
+      <c r="Q5" s="18"/>
       <c r="R5" s="12" t="s">
         <v>7</v>
       </c>
@@ -1015,14 +1074,14 @@
       <c r="T5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="U5" s="18" t="s">
+      <c r="U5" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="V5" s="18"/>
+      <c r="V5" s="20"/>
       <c r="W5" s="13">
         <v>496</v>
       </c>
-      <c r="Y5" s="16"/>
+      <c r="Y5" s="18"/>
       <c r="Z5" s="14" t="s">
         <v>7</v>
       </c>
@@ -1032,16 +1091,33 @@
       <c r="AB5" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="AC5" s="18" t="s">
+      <c r="AC5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="AD5" s="18"/>
+      <c r="AD5" s="20"/>
       <c r="AE5" s="15">
         <v>496</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI5" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK5" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="17">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
@@ -1051,15 +1127,15 @@
       <c r="D6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="18"/>
+      <c r="E6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="20"/>
       <c r="G6" s="10">
         <v>504</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="19"/>
+      <c r="I6" s="22"/>
       <c r="J6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1069,14 +1145,14 @@
       <c r="L6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="20"/>
+      <c r="M6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="21"/>
       <c r="O6" s="3">
         <v>504</v>
       </c>
-      <c r="Q6" s="16"/>
+      <c r="Q6" s="18"/>
       <c r="R6" s="12" t="s">
         <v>8</v>
       </c>
@@ -1086,14 +1162,14 @@
       <c r="T6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="V6" s="18"/>
+      <c r="U6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="V6" s="20"/>
       <c r="W6" s="13">
         <v>504</v>
       </c>
-      <c r="Y6" s="16"/>
+      <c r="Y6" s="18"/>
       <c r="Z6" s="14" t="s">
         <v>8</v>
       </c>
@@ -1103,16 +1179,33 @@
       <c r="AB6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AC6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD6" s="18"/>
+      <c r="AC6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="20"/>
       <c r="AE6" s="15">
         <v>504</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="AG6" s="18"/>
+      <c r="AH6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL6" s="20"/>
+      <c r="AM6" s="17">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -1120,85 +1213,105 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="Q7" s="16"/>
+      <c r="Q7" s="18"/>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
       <c r="W7" s="13"/>
-      <c r="Y7" s="16"/>
+      <c r="Y7" s="18"/>
       <c r="Z7" s="14"/>
       <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="15"/>
       <c r="AE7" s="15"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="16"/>
+      <c r="AI7" s="16"/>
+      <c r="AJ7" s="16"/>
+      <c r="AK7" s="17"/>
+      <c r="AL7" s="17"/>
+      <c r="AM7" s="17"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
       <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="10">
         <v>1000</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="20"/>
+      <c r="N8" s="21"/>
       <c r="O8" s="3">
         <v>1000</v>
       </c>
-      <c r="Q8" s="16"/>
+      <c r="Q8" s="18"/>
       <c r="R8" s="12" t="s">
         <v>21</v>
       </c>
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
-      <c r="U8" s="18" t="s">
+      <c r="U8" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="V8" s="18"/>
+      <c r="V8" s="20"/>
       <c r="W8" s="13">
         <v>1000</v>
       </c>
-      <c r="Y8" s="16"/>
+      <c r="Y8" s="18"/>
       <c r="Z8" s="14" t="s">
         <v>21</v>
       </c>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
-      <c r="AC8" s="18" t="s">
+      <c r="AC8" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="AD8" s="18"/>
+      <c r="AD8" s="20"/>
       <c r="AE8" s="15">
         <v>1000</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI8" s="16"/>
+      <c r="AJ8" s="16"/>
+      <c r="AK8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL8" s="20"/>
+      <c r="AM8" s="17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
       <c r="B9" s="9" t="s">
         <v>22</v>
       </c>
@@ -1208,15 +1321,15 @@
       <c r="D9" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="10">
         <v>1000</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1226,14 +1339,14 @@
       <c r="L9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M9" s="20" t="s">
+      <c r="M9" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="N9" s="20"/>
+      <c r="N9" s="21"/>
       <c r="O9" s="3">
         <v>1000</v>
       </c>
-      <c r="Q9" s="16"/>
+      <c r="Q9" s="18"/>
       <c r="R9" s="12" t="s">
         <v>22</v>
       </c>
@@ -1243,14 +1356,14 @@
       <c r="T9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="U9" s="18" t="s">
+      <c r="U9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="V9" s="18"/>
+      <c r="V9" s="20"/>
       <c r="W9" s="13">
         <v>1000</v>
       </c>
-      <c r="Y9" s="16"/>
+      <c r="Y9" s="18"/>
       <c r="Z9" s="14" t="s">
         <v>22</v>
       </c>
@@ -1260,16 +1373,33 @@
       <c r="AB9" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="AC9" s="18" t="s">
+      <c r="AC9" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="AD9" s="18"/>
+      <c r="AD9" s="20"/>
       <c r="AE9" s="15">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ9" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
       <c r="B10" s="9" t="s">
         <v>23</v>
       </c>
@@ -1279,15 +1409,15 @@
       <c r="D10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="10">
         <v>1000</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="19"/>
+      <c r="I10" s="22"/>
       <c r="J10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1297,14 +1427,14 @@
       <c r="L10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="20" t="s">
+      <c r="M10" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="20"/>
+      <c r="N10" s="21"/>
       <c r="O10" s="3">
         <v>1000</v>
       </c>
-      <c r="Q10" s="16"/>
+      <c r="Q10" s="18"/>
       <c r="R10" s="12" t="s">
         <v>23</v>
       </c>
@@ -1314,14 +1444,14 @@
       <c r="T10" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="U10" s="18" t="s">
+      <c r="U10" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="V10" s="18"/>
+      <c r="V10" s="20"/>
       <c r="W10" s="13">
         <v>1000</v>
       </c>
-      <c r="Y10" s="16"/>
+      <c r="Y10" s="18"/>
       <c r="Z10" s="14" t="s">
         <v>23</v>
       </c>
@@ -1331,15 +1461,32 @@
       <c r="AB10" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="AC10" s="18" t="s">
+      <c r="AC10" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="AD10" s="18"/>
+      <c r="AD10" s="20"/>
       <c r="AE10" s="15">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AG10" s="18"/>
+      <c r="AH10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1370,8 +1517,8 @@
       <c r="AD11" s="14"/>
       <c r="AE11" s="14"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -1383,15 +1530,15 @@
       <c r="D12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="22" t="s">
         <v>10</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -1403,14 +1550,14 @@
       <c r="L12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="M12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="N12" s="20"/>
+      <c r="N12" s="21"/>
       <c r="O12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q12" s="16" t="s">
+      <c r="Q12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="R12" s="12" t="s">
@@ -1422,14 +1569,14 @@
       <c r="T12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="U12" s="18" t="s">
+      <c r="U12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="V12" s="18"/>
+      <c r="V12" s="20"/>
       <c r="W12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="Y12" s="16" t="s">
+      <c r="Y12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="Z12" s="14" t="s">
@@ -1441,16 +1588,16 @@
       <c r="AB12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AC12" s="18" t="s">
+      <c r="AC12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AD12" s="18"/>
+      <c r="AD12" s="20"/>
       <c r="AE12" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
       <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
@@ -1460,15 +1607,15 @@
       <c r="D13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="10">
         <v>498</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="19"/>
+      <c r="I13" s="22"/>
       <c r="J13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1478,14 +1625,14 @@
       <c r="L13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="M13" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N13" s="20"/>
+      <c r="N13" s="21"/>
       <c r="O13" s="3">
         <v>498</v>
       </c>
-      <c r="Q13" s="16"/>
+      <c r="Q13" s="18"/>
       <c r="R13" s="12" t="s">
         <v>6</v>
       </c>
@@ -1495,14 +1642,14 @@
       <c r="T13" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="U13" s="18" t="s">
+      <c r="U13" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="V13" s="18"/>
+      <c r="V13" s="20"/>
       <c r="W13" s="13">
         <v>498</v>
       </c>
-      <c r="Y13" s="16"/>
+      <c r="Y13" s="18"/>
       <c r="Z13" s="14" t="s">
         <v>6</v>
       </c>
@@ -1512,16 +1659,16 @@
       <c r="AB13" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="AC13" s="18" t="s">
+      <c r="AC13" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="AD13" s="18"/>
+      <c r="AD13" s="20"/>
       <c r="AE13" s="15">
         <v>498</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
       <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
@@ -1531,15 +1678,15 @@
       <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="10">
         <v>498</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="19"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1549,14 +1696,14 @@
       <c r="L14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="20" t="s">
+      <c r="M14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="20"/>
+      <c r="N14" s="21"/>
       <c r="O14" s="3">
         <v>498</v>
       </c>
-      <c r="Q14" s="16"/>
+      <c r="Q14" s="18"/>
       <c r="R14" s="12" t="s">
         <v>7</v>
       </c>
@@ -1566,14 +1713,14 @@
       <c r="T14" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="U14" s="18" t="s">
+      <c r="U14" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="V14" s="18"/>
+      <c r="V14" s="20"/>
       <c r="W14" s="13">
         <v>498</v>
       </c>
-      <c r="Y14" s="16"/>
+      <c r="Y14" s="18"/>
       <c r="Z14" s="14" t="s">
         <v>7</v>
       </c>
@@ -1583,16 +1730,16 @@
       <c r="AB14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AC14" s="18" t="s">
+      <c r="AC14" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AD14" s="18"/>
+      <c r="AD14" s="20"/>
       <c r="AE14" s="15">
         <v>498</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
       <c r="B15" s="9" t="s">
         <v>8</v>
       </c>
@@ -1602,15 +1749,15 @@
       <c r="D15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="18"/>
+      <c r="E15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="20"/>
       <c r="G15" s="10">
         <v>0</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1620,14 +1767,14 @@
       <c r="L15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M15" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15" s="20"/>
+      <c r="M15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="21"/>
       <c r="O15" s="3">
         <v>0</v>
       </c>
-      <c r="Q15" s="16"/>
+      <c r="Q15" s="18"/>
       <c r="R15" s="12" t="s">
         <v>8</v>
       </c>
@@ -1637,14 +1784,14 @@
       <c r="T15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="U15" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="V15" s="18"/>
+      <c r="U15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="V15" s="20"/>
       <c r="W15" s="13">
         <v>0</v>
       </c>
-      <c r="Y15" s="16"/>
+      <c r="Y15" s="18"/>
       <c r="Z15" s="14" t="s">
         <v>8</v>
       </c>
@@ -1654,16 +1801,16 @@
       <c r="AB15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AC15" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD15" s="18"/>
+      <c r="AC15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD15" s="20"/>
       <c r="AE15" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1671,21 +1818,21 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="19"/>
+      <c r="I16" s="22"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
-      <c r="Q16" s="16"/>
+      <c r="Q16" s="18"/>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
       <c r="W16" s="13"/>
-      <c r="Y16" s="16"/>
+      <c r="Y16" s="18"/>
       <c r="Z16" s="14"/>
       <c r="AA16" s="14"/>
       <c r="AB16" s="14"/>
@@ -1694,62 +1841,62 @@
       <c r="AE16" s="15"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="10">
         <v>996</v>
       </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="20" t="s">
+      <c r="M17" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="20"/>
+      <c r="N17" s="21"/>
       <c r="O17" s="3">
         <v>996</v>
       </c>
-      <c r="Q17" s="16"/>
+      <c r="Q17" s="18"/>
       <c r="R17" s="12" t="s">
         <v>21</v>
       </c>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
-      <c r="U17" s="18" t="s">
+      <c r="U17" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="V17" s="18"/>
+      <c r="V17" s="20"/>
       <c r="W17" s="13">
         <v>996</v>
       </c>
-      <c r="Y17" s="16"/>
+      <c r="Y17" s="18"/>
       <c r="Z17" s="14" t="s">
         <v>21</v>
       </c>
       <c r="AA17" s="14"/>
       <c r="AB17" s="14"/>
-      <c r="AC17" s="18" t="s">
+      <c r="AC17" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="AD17" s="18"/>
+      <c r="AD17" s="20"/>
       <c r="AE17" s="15">
         <v>996</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="9" t="s">
         <v>22</v>
       </c>
@@ -1759,15 +1906,15 @@
       <c r="D18" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="10">
         <v>996</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="19"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1777,14 +1924,14 @@
       <c r="L18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M18" s="20" t="s">
+      <c r="M18" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N18" s="20"/>
+      <c r="N18" s="21"/>
       <c r="O18" s="3">
         <v>996</v>
       </c>
-      <c r="Q18" s="16"/>
+      <c r="Q18" s="18"/>
       <c r="R18" s="12" t="s">
         <v>22</v>
       </c>
@@ -1794,14 +1941,14 @@
       <c r="T18" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="U18" s="18" t="s">
+      <c r="U18" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="V18" s="18"/>
+      <c r="V18" s="20"/>
       <c r="W18" s="13">
         <v>996</v>
       </c>
-      <c r="Y18" s="16"/>
+      <c r="Y18" s="18"/>
       <c r="Z18" s="14" t="s">
         <v>22</v>
       </c>
@@ -1811,16 +1958,16 @@
       <c r="AB18" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="AC18" s="18" t="s">
+      <c r="AC18" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="AD18" s="18"/>
+      <c r="AD18" s="20"/>
       <c r="AE18" s="15">
         <v>996</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="9" t="s">
         <v>23</v>
       </c>
@@ -1830,15 +1977,15 @@
       <c r="D19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="10">
         <v>996</v>
       </c>
       <c r="H19" s="2"/>
-      <c r="I19" s="19"/>
+      <c r="I19" s="22"/>
       <c r="J19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1848,14 +1995,14 @@
       <c r="L19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="M19" s="20" t="s">
+      <c r="M19" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="N19" s="20"/>
+      <c r="N19" s="21"/>
       <c r="O19" s="3">
         <v>996</v>
       </c>
-      <c r="Q19" s="16"/>
+      <c r="Q19" s="18"/>
       <c r="R19" s="12" t="s">
         <v>23</v>
       </c>
@@ -1865,14 +2012,14 @@
       <c r="T19" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="U19" s="18" t="s">
+      <c r="U19" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="V19" s="18"/>
+      <c r="V19" s="20"/>
       <c r="W19" s="13">
         <v>996</v>
       </c>
-      <c r="Y19" s="16"/>
+      <c r="Y19" s="18"/>
       <c r="Z19" s="14" t="s">
         <v>23</v>
       </c>
@@ -1882,10 +2029,10 @@
       <c r="AB19" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AC19" s="18" t="s">
+      <c r="AC19" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="AD19" s="18"/>
+      <c r="AD19" s="20"/>
       <c r="AE19" s="15">
         <v>996</v>
       </c>
@@ -1922,7 +2069,7 @@
       <c r="AE20" s="14"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -1934,15 +2081,15 @@
       <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="22" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -1954,14 +2101,14 @@
       <c r="L21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="20" t="s">
+      <c r="M21" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="N21" s="20"/>
+      <c r="N21" s="21"/>
       <c r="O21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" s="16" t="s">
+      <c r="Q21" s="18" t="s">
         <v>11</v>
       </c>
       <c r="R21" s="12" t="s">
@@ -1973,14 +2120,14 @@
       <c r="T21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="U21" s="18" t="s">
+      <c r="U21" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="V21" s="18"/>
+      <c r="V21" s="20"/>
       <c r="W21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="Y21" s="16" t="s">
+      <c r="Y21" s="18" t="s">
         <v>11</v>
       </c>
       <c r="Z21" s="14" t="s">
@@ -1992,16 +2139,16 @@
       <c r="AB21" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AC21" s="18" t="s">
+      <c r="AC21" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AD21" s="18"/>
+      <c r="AD21" s="20"/>
       <c r="AE21" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="9" t="s">
         <v>6</v>
       </c>
@@ -2011,15 +2158,15 @@
       <c r="D22" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="10">
         <v>500</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="19"/>
+      <c r="I22" s="22"/>
       <c r="J22" s="2" t="s">
         <v>6</v>
       </c>
@@ -2029,14 +2176,14 @@
       <c r="L22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="M22" s="20" t="s">
+      <c r="M22" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N22" s="20"/>
+      <c r="N22" s="21"/>
       <c r="O22" s="3">
         <v>500</v>
       </c>
-      <c r="Q22" s="16"/>
+      <c r="Q22" s="18"/>
       <c r="R22" s="12" t="s">
         <v>6</v>
       </c>
@@ -2046,14 +2193,14 @@
       <c r="T22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="U22" s="18" t="s">
+      <c r="U22" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="V22" s="18"/>
+      <c r="V22" s="20"/>
       <c r="W22" s="13">
         <v>500</v>
       </c>
-      <c r="Y22" s="16"/>
+      <c r="Y22" s="18"/>
       <c r="Z22" s="14" t="s">
         <v>6</v>
       </c>
@@ -2063,16 +2210,16 @@
       <c r="AB22" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="AC22" s="18" t="s">
+      <c r="AC22" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="AD22" s="18"/>
+      <c r="AD22" s="20"/>
       <c r="AE22" s="15">
         <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="9" t="s">
         <v>7</v>
       </c>
@@ -2082,15 +2229,15 @@
       <c r="D23" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="10">
         <v>500</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="19"/>
+      <c r="I23" s="22"/>
       <c r="J23" s="2" t="s">
         <v>7</v>
       </c>
@@ -2100,14 +2247,14 @@
       <c r="L23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M23" s="20" t="s">
+      <c r="M23" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N23" s="20"/>
+      <c r="N23" s="21"/>
       <c r="O23" s="3">
         <v>500</v>
       </c>
-      <c r="Q23" s="16"/>
+      <c r="Q23" s="18"/>
       <c r="R23" s="12" t="s">
         <v>7</v>
       </c>
@@ -2117,14 +2264,14 @@
       <c r="T23" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="U23" s="18" t="s">
+      <c r="U23" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="V23" s="18"/>
+      <c r="V23" s="20"/>
       <c r="W23" s="13">
         <v>500</v>
       </c>
-      <c r="Y23" s="16"/>
+      <c r="Y23" s="18"/>
       <c r="Z23" s="14" t="s">
         <v>7</v>
       </c>
@@ -2134,16 +2281,16 @@
       <c r="AB23" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="AC23" s="18" t="s">
+      <c r="AC23" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="AD23" s="18"/>
+      <c r="AD23" s="20"/>
       <c r="AE23" s="15">
         <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="9" t="s">
         <v>8</v>
       </c>
@@ -2153,13 +2300,13 @@
       <c r="D24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="18"/>
+      <c r="E24" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="20"/>
       <c r="G24" s="10"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="19"/>
+      <c r="I24" s="22"/>
       <c r="J24" s="2" t="s">
         <v>8</v>
       </c>
@@ -2169,12 +2316,12 @@
       <c r="L24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N24" s="20"/>
+      <c r="M24" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="21"/>
       <c r="O24" s="3"/>
-      <c r="Q24" s="16"/>
+      <c r="Q24" s="18"/>
       <c r="R24" s="12" t="s">
         <v>8</v>
       </c>
@@ -2184,12 +2331,12 @@
       <c r="T24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="U24" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="V24" s="18"/>
+      <c r="U24" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="V24" s="20"/>
       <c r="W24" s="13"/>
-      <c r="Y24" s="16"/>
+      <c r="Y24" s="18"/>
       <c r="Z24" s="14" t="s">
         <v>8</v>
       </c>
@@ -2199,14 +2346,14 @@
       <c r="AB24" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AC24" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD24" s="18"/>
+      <c r="AC24" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD24" s="20"/>
       <c r="AE24" s="15"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2214,21 +2361,21 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="19"/>
+      <c r="I25" s="22"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="Q25" s="16"/>
+      <c r="Q25" s="18"/>
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
       <c r="T25" s="12"/>
       <c r="U25" s="13"/>
       <c r="V25" s="13"/>
       <c r="W25" s="13"/>
-      <c r="Y25" s="16"/>
+      <c r="Y25" s="18"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="14"/>
       <c r="AB25" s="14"/>
@@ -2237,62 +2384,62 @@
       <c r="AE25" s="15"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="10">
         <v>1000</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="19"/>
+      <c r="I26" s="22"/>
       <c r="J26" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="20" t="s">
+      <c r="M26" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="N26" s="20"/>
+      <c r="N26" s="21"/>
       <c r="O26" s="3">
         <v>1000</v>
       </c>
-      <c r="Q26" s="16"/>
+      <c r="Q26" s="18"/>
       <c r="R26" s="12" t="s">
         <v>21</v>
       </c>
       <c r="S26" s="12"/>
       <c r="T26" s="12"/>
-      <c r="U26" s="18" t="s">
+      <c r="U26" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="V26" s="18"/>
+      <c r="V26" s="20"/>
       <c r="W26" s="13">
         <v>1000</v>
       </c>
-      <c r="Y26" s="16"/>
+      <c r="Y26" s="18"/>
       <c r="Z26" s="14" t="s">
         <v>21</v>
       </c>
       <c r="AA26" s="14"/>
       <c r="AB26" s="14"/>
-      <c r="AC26" s="18" t="s">
+      <c r="AC26" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="AD26" s="18"/>
+      <c r="AD26" s="20"/>
       <c r="AE26" s="15">
         <v>1000</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="9" t="s">
         <v>22</v>
       </c>
@@ -2302,15 +2449,15 @@
       <c r="D27" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="10">
         <v>1000</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="19"/>
+      <c r="I27" s="22"/>
       <c r="J27" s="2" t="s">
         <v>22</v>
       </c>
@@ -2320,14 +2467,14 @@
       <c r="L27" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M27" s="20" t="s">
+      <c r="M27" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N27" s="20"/>
+      <c r="N27" s="21"/>
       <c r="O27" s="3">
         <v>1000</v>
       </c>
-      <c r="Q27" s="16"/>
+      <c r="Q27" s="18"/>
       <c r="R27" s="12" t="s">
         <v>22</v>
       </c>
@@ -2337,14 +2484,14 @@
       <c r="T27" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="U27" s="18" t="s">
+      <c r="U27" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="V27" s="18"/>
+      <c r="V27" s="20"/>
       <c r="W27" s="13">
         <v>1000</v>
       </c>
-      <c r="Y27" s="16"/>
+      <c r="Y27" s="18"/>
       <c r="Z27" s="14" t="s">
         <v>22</v>
       </c>
@@ -2354,16 +2501,16 @@
       <c r="AB27" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="AC27" s="18" t="s">
+      <c r="AC27" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="AD27" s="18"/>
+      <c r="AD27" s="20"/>
       <c r="AE27" s="15">
         <v>1000</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="9" t="s">
         <v>23</v>
       </c>
@@ -2373,15 +2520,15 @@
       <c r="D28" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="18"/>
+      <c r="F28" s="20"/>
       <c r="G28" s="10">
         <v>1000</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="19"/>
+      <c r="I28" s="22"/>
       <c r="J28" s="2" t="s">
         <v>23</v>
       </c>
@@ -2391,14 +2538,14 @@
       <c r="L28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M28" s="20" t="s">
+      <c r="M28" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N28" s="20"/>
+      <c r="N28" s="21"/>
       <c r="O28" s="3">
         <v>1000</v>
       </c>
-      <c r="Q28" s="16"/>
+      <c r="Q28" s="18"/>
       <c r="R28" s="12" t="s">
         <v>23</v>
       </c>
@@ -2408,14 +2555,14 @@
       <c r="T28" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="U28" s="18" t="s">
+      <c r="U28" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="V28" s="18"/>
+      <c r="V28" s="20"/>
       <c r="W28" s="13">
         <v>1000</v>
       </c>
-      <c r="Y28" s="16"/>
+      <c r="Y28" s="18"/>
       <c r="Z28" s="14" t="s">
         <v>23</v>
       </c>
@@ -2425,10 +2572,10 @@
       <c r="AB28" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="AC28" s="18" t="s">
+      <c r="AC28" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="AD28" s="18"/>
+      <c r="AD28" s="20"/>
       <c r="AE28" s="15">
         <v>1000</v>
       </c>
@@ -2465,7 +2612,7 @@
       <c r="AE29" s="14"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -2477,15 +2624,15 @@
       <c r="D30" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="17"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30" s="19" t="s">
+      <c r="I30" s="22" t="s">
         <v>12</v>
       </c>
       <c r="J30" s="4" t="s">
@@ -2497,14 +2644,14 @@
       <c r="L30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M30" s="17" t="s">
+      <c r="M30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N30" s="17"/>
+      <c r="N30" s="19"/>
       <c r="O30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="16" t="s">
+      <c r="Q30" s="18" t="s">
         <v>12</v>
       </c>
       <c r="R30" s="12" t="s">
@@ -2516,14 +2663,14 @@
       <c r="T30" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="U30" s="17" t="s">
+      <c r="U30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="V30" s="17"/>
+      <c r="V30" s="19"/>
       <c r="W30" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="Y30" s="16" t="s">
+      <c r="Y30" s="18" t="s">
         <v>12</v>
       </c>
       <c r="Z30" s="14" t="s">
@@ -2535,16 +2682,16 @@
       <c r="AB30" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AC30" s="17" t="s">
+      <c r="AC30" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AD30" s="17"/>
+      <c r="AD30" s="19"/>
       <c r="AE30" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="9" t="s">
         <v>6</v>
       </c>
@@ -2554,15 +2701,15 @@
       <c r="D31" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="F31" s="18"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="9">
         <v>167</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="19"/>
+      <c r="I31" s="22"/>
       <c r="J31" s="4" t="s">
         <v>6</v>
       </c>
@@ -2572,14 +2719,14 @@
       <c r="L31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M31" s="18" t="s">
+      <c r="M31" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="N31" s="18"/>
+      <c r="N31" s="20"/>
       <c r="O31" s="4">
         <v>167</v>
       </c>
-      <c r="Q31" s="16"/>
+      <c r="Q31" s="18"/>
       <c r="R31" s="12" t="s">
         <v>6</v>
       </c>
@@ -2589,14 +2736,14 @@
       <c r="T31" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="U31" s="18" t="s">
+      <c r="U31" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="V31" s="18"/>
+      <c r="V31" s="20"/>
       <c r="W31" s="12">
         <v>167</v>
       </c>
-      <c r="Y31" s="16"/>
+      <c r="Y31" s="18"/>
       <c r="Z31" s="14" t="s">
         <v>6</v>
       </c>
@@ -2606,16 +2753,16 @@
       <c r="AB31" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="AC31" s="18" t="s">
+      <c r="AC31" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AD31" s="18"/>
+      <c r="AD31" s="20"/>
       <c r="AE31" s="14">
         <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="9" t="s">
         <v>7</v>
       </c>
@@ -2625,15 +2772,15 @@
       <c r="D32" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="F32" s="18"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="9">
         <v>769</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="19"/>
+      <c r="I32" s="22"/>
       <c r="J32" s="4" t="s">
         <v>7</v>
       </c>
@@ -2643,14 +2790,14 @@
       <c r="L32" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M32" s="18" t="s">
+      <c r="M32" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="N32" s="18"/>
+      <c r="N32" s="20"/>
       <c r="O32" s="4">
         <v>769</v>
       </c>
-      <c r="Q32" s="16"/>
+      <c r="Q32" s="18"/>
       <c r="R32" s="12" t="s">
         <v>7</v>
       </c>
@@ -2660,14 +2807,14 @@
       <c r="T32" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="U32" s="18" t="s">
+      <c r="U32" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="V32" s="18"/>
+      <c r="V32" s="20"/>
       <c r="W32" s="12">
         <v>769</v>
       </c>
-      <c r="Y32" s="16"/>
+      <c r="Y32" s="18"/>
       <c r="Z32" s="14" t="s">
         <v>7</v>
       </c>
@@ -2677,16 +2824,16 @@
       <c r="AB32" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="AC32" s="18" t="s">
+      <c r="AC32" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="AD32" s="18"/>
+      <c r="AD32" s="20"/>
       <c r="AE32" s="14">
         <v>769</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="9" t="s">
         <v>8</v>
       </c>
@@ -2696,15 +2843,15 @@
       <c r="D33" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="18"/>
+      <c r="E33" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="20"/>
       <c r="G33" s="9">
         <v>0</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="19"/>
+      <c r="I33" s="22"/>
       <c r="J33" s="4" t="s">
         <v>8</v>
       </c>
@@ -2714,14 +2861,14 @@
       <c r="L33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M33" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="N33" s="18"/>
+      <c r="M33" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" s="20"/>
       <c r="O33" s="4">
         <v>0</v>
       </c>
-      <c r="Q33" s="16"/>
+      <c r="Q33" s="18"/>
       <c r="R33" s="12" t="s">
         <v>8</v>
       </c>
@@ -2731,14 +2878,14 @@
       <c r="T33" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="U33" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="V33" s="18"/>
+      <c r="U33" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="V33" s="20"/>
       <c r="W33" s="12">
         <v>0</v>
       </c>
-      <c r="Y33" s="16"/>
+      <c r="Y33" s="18"/>
       <c r="Z33" s="14" t="s">
         <v>8</v>
       </c>
@@ -2748,16 +2895,16 @@
       <c r="AB33" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AC33" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD33" s="18"/>
+      <c r="AC33" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD33" s="20"/>
       <c r="AE33" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2765,21 +2912,21 @@
       <c r="F34" s="10"/>
       <c r="G34" s="9"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="19"/>
+      <c r="I34" s="22"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="4"/>
-      <c r="Q34" s="16"/>
+      <c r="Q34" s="18"/>
       <c r="R34" s="12"/>
       <c r="S34" s="12"/>
       <c r="T34" s="12"/>
       <c r="U34" s="13"/>
       <c r="V34" s="13"/>
       <c r="W34" s="12"/>
-      <c r="Y34" s="16"/>
+      <c r="Y34" s="18"/>
       <c r="Z34" s="14"/>
       <c r="AA34" s="14"/>
       <c r="AB34" s="14"/>
@@ -2788,62 +2935,62 @@
       <c r="AE34" s="14"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="18"/>
+      <c r="F35" s="20"/>
       <c r="G35" s="9">
         <v>936</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="19"/>
+      <c r="I35" s="22"/>
       <c r="J35" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="18" t="s">
+      <c r="M35" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="N35" s="18"/>
+      <c r="N35" s="20"/>
       <c r="O35" s="4">
         <v>936</v>
       </c>
-      <c r="Q35" s="16"/>
+      <c r="Q35" s="18"/>
       <c r="R35" s="12" t="s">
         <v>21</v>
       </c>
       <c r="S35" s="12"/>
       <c r="T35" s="12"/>
-      <c r="U35" s="18" t="s">
+      <c r="U35" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="V35" s="18"/>
+      <c r="V35" s="20"/>
       <c r="W35" s="12">
         <v>936</v>
       </c>
-      <c r="Y35" s="16"/>
+      <c r="Y35" s="18"/>
       <c r="Z35" s="14" t="s">
         <v>21</v>
       </c>
       <c r="AA35" s="14"/>
       <c r="AB35" s="14"/>
-      <c r="AC35" s="18" t="s">
+      <c r="AC35" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="AD35" s="18"/>
+      <c r="AD35" s="20"/>
       <c r="AE35" s="14">
         <v>936</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="9" t="s">
         <v>22</v>
       </c>
@@ -2853,15 +3000,15 @@
       <c r="D36" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="18"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="9">
         <v>936</v>
       </c>
       <c r="H36" s="2"/>
-      <c r="I36" s="19"/>
+      <c r="I36" s="22"/>
       <c r="J36" s="2" t="s">
         <v>22</v>
       </c>
@@ -2871,14 +3018,14 @@
       <c r="L36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M36" s="18" t="s">
+      <c r="M36" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="N36" s="18"/>
+      <c r="N36" s="20"/>
       <c r="O36" s="4">
         <v>936</v>
       </c>
-      <c r="Q36" s="16"/>
+      <c r="Q36" s="18"/>
       <c r="R36" s="12" t="s">
         <v>22</v>
       </c>
@@ -2888,14 +3035,14 @@
       <c r="T36" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="U36" s="18" t="s">
+      <c r="U36" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="V36" s="18"/>
+      <c r="V36" s="20"/>
       <c r="W36" s="12">
         <v>936</v>
       </c>
-      <c r="Y36" s="16"/>
+      <c r="Y36" s="18"/>
       <c r="Z36" s="14" t="s">
         <v>22</v>
       </c>
@@ -2905,16 +3052,16 @@
       <c r="AB36" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AC36" s="18" t="s">
+      <c r="AC36" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="AD36" s="18"/>
+      <c r="AD36" s="20"/>
       <c r="AE36" s="14">
         <v>936</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="9" t="s">
         <v>23</v>
       </c>
@@ -2924,15 +3071,15 @@
       <c r="D37" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="18"/>
+      <c r="F37" s="20"/>
       <c r="G37" s="9">
         <v>936</v>
       </c>
       <c r="H37" s="2"/>
-      <c r="I37" s="19"/>
+      <c r="I37" s="22"/>
       <c r="J37" s="2" t="s">
         <v>23</v>
       </c>
@@ -2942,14 +3089,14 @@
       <c r="L37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M37" s="18" t="s">
+      <c r="M37" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="N37" s="18"/>
+      <c r="N37" s="20"/>
       <c r="O37" s="4">
         <v>936</v>
       </c>
-      <c r="Q37" s="16"/>
+      <c r="Q37" s="18"/>
       <c r="R37" s="12" t="s">
         <v>23</v>
       </c>
@@ -2959,14 +3106,14 @@
       <c r="T37" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="U37" s="18" t="s">
+      <c r="U37" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="V37" s="18"/>
+      <c r="V37" s="20"/>
       <c r="W37" s="12">
         <v>936</v>
       </c>
-      <c r="Y37" s="16"/>
+      <c r="Y37" s="18"/>
       <c r="Z37" s="14" t="s">
         <v>23</v>
       </c>
@@ -2976,10 +3123,10 @@
       <c r="AB37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="AC37" s="18" t="s">
+      <c r="AC37" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="AD37" s="18"/>
+      <c r="AD37" s="20"/>
       <c r="AE37" s="14">
         <v>936</v>
       </c>
@@ -3016,7 +3163,7 @@
       <c r="AE38" s="14"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -3028,15 +3175,15 @@
       <c r="D39" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="18"/>
+      <c r="F39" s="20"/>
       <c r="G39" s="10" t="s">
         <v>17</v>
       </c>
       <c r="H39" s="2"/>
-      <c r="I39" s="19" t="s">
+      <c r="I39" s="22" t="s">
         <v>13</v>
       </c>
       <c r="J39" s="2" t="s">
@@ -3048,14 +3195,14 @@
       <c r="L39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M39" s="20" t="s">
+      <c r="M39" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="N39" s="20"/>
+      <c r="N39" s="21"/>
       <c r="O39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q39" s="16" t="s">
+      <c r="Q39" s="18" t="s">
         <v>13</v>
       </c>
       <c r="R39" s="12" t="s">
@@ -3067,14 +3214,14 @@
       <c r="T39" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="U39" s="18" t="s">
+      <c r="U39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="V39" s="18"/>
+      <c r="V39" s="20"/>
       <c r="W39" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="Y39" s="16" t="s">
+      <c r="Y39" s="18" t="s">
         <v>13</v>
       </c>
       <c r="Z39" s="14" t="s">
@@ -3086,16 +3233,16 @@
       <c r="AB39" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AC39" s="18" t="s">
+      <c r="AC39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AD39" s="18"/>
+      <c r="AD39" s="20"/>
       <c r="AE39" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="9" t="s">
         <v>6</v>
       </c>
@@ -3105,15 +3252,15 @@
       <c r="D40" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F40" s="18"/>
+      <c r="F40" s="20"/>
       <c r="G40" s="10">
         <v>483</v>
       </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="19"/>
+      <c r="I40" s="22"/>
       <c r="J40" s="2" t="s">
         <v>6</v>
       </c>
@@ -3123,14 +3270,14 @@
       <c r="L40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M40" s="20" t="s">
+      <c r="M40" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N40" s="20"/>
+      <c r="N40" s="21"/>
       <c r="O40" s="3">
         <v>483</v>
       </c>
-      <c r="Q40" s="16"/>
+      <c r="Q40" s="18"/>
       <c r="R40" s="12" t="s">
         <v>6</v>
       </c>
@@ -3140,14 +3287,14 @@
       <c r="T40" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="U40" s="18" t="s">
+      <c r="U40" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="V40" s="18"/>
+      <c r="V40" s="20"/>
       <c r="W40" s="13">
         <v>483</v>
       </c>
-      <c r="Y40" s="16"/>
+      <c r="Y40" s="18"/>
       <c r="Z40" s="14" t="s">
         <v>6</v>
       </c>
@@ -3157,16 +3304,16 @@
       <c r="AB40" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AC40" s="18" t="s">
+      <c r="AC40" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="AD40" s="18"/>
+      <c r="AD40" s="20"/>
       <c r="AE40" s="15">
         <v>483</v>
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
@@ -3176,15 +3323,15 @@
       <c r="D41" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="18"/>
+      <c r="F41" s="20"/>
       <c r="G41" s="10">
         <v>517</v>
       </c>
       <c r="H41" s="2"/>
-      <c r="I41" s="19"/>
+      <c r="I41" s="22"/>
       <c r="J41" s="2" t="s">
         <v>7</v>
       </c>
@@ -3194,14 +3341,14 @@
       <c r="L41" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M41" s="20" t="s">
+      <c r="M41" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="N41" s="20"/>
+      <c r="N41" s="21"/>
       <c r="O41" s="3">
         <v>517</v>
       </c>
-      <c r="Q41" s="16"/>
+      <c r="Q41" s="18"/>
       <c r="R41" s="12" t="s">
         <v>7</v>
       </c>
@@ -3211,14 +3358,14 @@
       <c r="T41" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="U41" s="18" t="s">
+      <c r="U41" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="V41" s="18"/>
+      <c r="V41" s="20"/>
       <c r="W41" s="13">
         <v>517</v>
       </c>
-      <c r="Y41" s="16"/>
+      <c r="Y41" s="18"/>
       <c r="Z41" s="14" t="s">
         <v>7</v>
       </c>
@@ -3228,16 +3375,16 @@
       <c r="AB41" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AC41" s="18" t="s">
+      <c r="AC41" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="AD41" s="18"/>
+      <c r="AD41" s="20"/>
       <c r="AE41" s="15">
         <v>517</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="9" t="s">
         <v>8</v>
       </c>
@@ -3247,15 +3394,15 @@
       <c r="D42" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="18"/>
+      <c r="E42" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="20"/>
       <c r="G42" s="10">
         <v>0</v>
       </c>
       <c r="H42" s="2"/>
-      <c r="I42" s="19"/>
+      <c r="I42" s="22"/>
       <c r="J42" s="2" t="s">
         <v>8</v>
       </c>
@@ -3265,14 +3412,14 @@
       <c r="L42" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N42" s="20"/>
+      <c r="M42" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" s="21"/>
       <c r="O42" s="3">
         <v>0</v>
       </c>
-      <c r="Q42" s="16"/>
+      <c r="Q42" s="18"/>
       <c r="R42" s="12" t="s">
         <v>8</v>
       </c>
@@ -3282,14 +3429,14 @@
       <c r="T42" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="U42" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="V42" s="18"/>
+      <c r="U42" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="V42" s="20"/>
       <c r="W42" s="13">
         <v>0</v>
       </c>
-      <c r="Y42" s="16"/>
+      <c r="Y42" s="18"/>
       <c r="Z42" s="14" t="s">
         <v>8</v>
       </c>
@@ -3299,16 +3446,16 @@
       <c r="AB42" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AC42" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD42" s="18"/>
+      <c r="AC42" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD42" s="20"/>
       <c r="AE42" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
@@ -3316,21 +3463,21 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="19"/>
+      <c r="I43" s="22"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
-      <c r="Q43" s="16"/>
+      <c r="Q43" s="18"/>
       <c r="R43" s="12"/>
       <c r="S43" s="12"/>
       <c r="T43" s="12"/>
       <c r="U43" s="13"/>
       <c r="V43" s="13"/>
       <c r="W43" s="13"/>
-      <c r="Y43" s="16"/>
+      <c r="Y43" s="18"/>
       <c r="Z43" s="14"/>
       <c r="AA43" s="14"/>
       <c r="AB43" s="14"/>
@@ -3339,62 +3486,62 @@
       <c r="AE43" s="15"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="18"/>
+      <c r="F44" s="20"/>
       <c r="G44" s="10">
         <v>1000</v>
       </c>
       <c r="H44" s="2"/>
-      <c r="I44" s="19"/>
+      <c r="I44" s="22"/>
       <c r="J44" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="20" t="s">
+      <c r="M44" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="N44" s="20"/>
+      <c r="N44" s="21"/>
       <c r="O44" s="3">
         <v>1000</v>
       </c>
-      <c r="Q44" s="16"/>
+      <c r="Q44" s="18"/>
       <c r="R44" s="12" t="s">
         <v>21</v>
       </c>
       <c r="S44" s="12"/>
       <c r="T44" s="12"/>
-      <c r="U44" s="18" t="s">
+      <c r="U44" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="V44" s="18"/>
+      <c r="V44" s="20"/>
       <c r="W44" s="13">
         <v>1000</v>
       </c>
-      <c r="Y44" s="16"/>
+      <c r="Y44" s="18"/>
       <c r="Z44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="AA44" s="14"/>
       <c r="AB44" s="14"/>
-      <c r="AC44" s="18" t="s">
+      <c r="AC44" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="AD44" s="18"/>
+      <c r="AD44" s="20"/>
       <c r="AE44" s="15">
         <v>1000</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="9" t="s">
         <v>22</v>
       </c>
@@ -3404,15 +3551,15 @@
       <c r="D45" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E45" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F45" s="18"/>
+      <c r="F45" s="20"/>
       <c r="G45" s="10">
         <v>1000</v>
       </c>
       <c r="H45" s="2"/>
-      <c r="I45" s="19"/>
+      <c r="I45" s="22"/>
       <c r="J45" s="2" t="s">
         <v>22</v>
       </c>
@@ -3422,14 +3569,14 @@
       <c r="L45" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M45" s="20" t="s">
+      <c r="M45" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="N45" s="20"/>
+      <c r="N45" s="21"/>
       <c r="O45" s="3">
         <v>1000</v>
       </c>
-      <c r="Q45" s="16"/>
+      <c r="Q45" s="18"/>
       <c r="R45" s="12" t="s">
         <v>22</v>
       </c>
@@ -3439,14 +3586,14 @@
       <c r="T45" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="U45" s="18" t="s">
+      <c r="U45" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="V45" s="18"/>
+      <c r="V45" s="20"/>
       <c r="W45" s="13">
         <v>1000</v>
       </c>
-      <c r="Y45" s="16"/>
+      <c r="Y45" s="18"/>
       <c r="Z45" s="14" t="s">
         <v>22</v>
       </c>
@@ -3456,16 +3603,16 @@
       <c r="AB45" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="AC45" s="18" t="s">
+      <c r="AC45" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AD45" s="18"/>
+      <c r="AD45" s="20"/>
       <c r="AE45" s="15">
         <v>1000</v>
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="9" t="s">
         <v>23</v>
       </c>
@@ -3475,15 +3622,15 @@
       <c r="D46" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="F46" s="18"/>
+      <c r="F46" s="20"/>
       <c r="G46" s="10">
         <v>1000</v>
       </c>
       <c r="H46" s="2"/>
-      <c r="I46" s="19"/>
+      <c r="I46" s="22"/>
       <c r="J46" s="2" t="s">
         <v>23</v>
       </c>
@@ -3493,14 +3640,14 @@
       <c r="L46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M46" s="20" t="s">
+      <c r="M46" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N46" s="20"/>
+      <c r="N46" s="21"/>
       <c r="O46" s="3">
         <v>1000</v>
       </c>
-      <c r="Q46" s="16"/>
+      <c r="Q46" s="18"/>
       <c r="R46" s="12" t="s">
         <v>23</v>
       </c>
@@ -3510,14 +3657,14 @@
       <c r="T46" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="U46" s="18" t="s">
+      <c r="U46" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="V46" s="18"/>
+      <c r="V46" s="20"/>
       <c r="W46" s="13">
         <v>1000</v>
       </c>
-      <c r="Y46" s="16"/>
+      <c r="Y46" s="18"/>
       <c r="Z46" s="14" t="s">
         <v>23</v>
       </c>
@@ -3527,10 +3674,10 @@
       <c r="AB46" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="AC46" s="18" t="s">
+      <c r="AC46" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="AD46" s="18"/>
+      <c r="AD46" s="20"/>
       <c r="AE46" s="15">
         <v>1000</v>
       </c>
@@ -3569,8 +3716,8 @@
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
       <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3578,8 +3725,8 @@
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
       <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3587,8 +3734,8 @@
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
       <c r="G55" s="5"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3596,8 +3743,8 @@
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
       <c r="G56" s="5"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3614,8 +3761,8 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
       <c r="G58" s="5"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3623,8 +3770,8 @@
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
       <c r="G59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3632,8 +3779,8 @@
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
       <c r="G60" s="5"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3650,8 +3797,8 @@
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
       <c r="G62" s="5"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3659,8 +3806,8 @@
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
       <c r="G63" s="5"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3668,8 +3815,8 @@
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
       <c r="G64" s="5"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3677,8 +3824,8 @@
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
       <c r="G65" s="5"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3695,8 +3842,8 @@
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
       <c r="G67" s="5"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3704,8 +3851,8 @@
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
       <c r="G68" s="5"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3713,8 +3860,8 @@
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
       <c r="G69" s="5"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3731,8 +3878,8 @@
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
       <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3740,8 +3887,8 @@
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
       <c r="G72" s="5"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3749,8 +3896,8 @@
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
       <c r="G73" s="5"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3758,8 +3905,8 @@
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
       <c r="G74" s="5"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3776,8 +3923,8 @@
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
       <c r="G76" s="5"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3785,8 +3932,8 @@
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3794,8 +3941,8 @@
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
       <c r="G78" s="5"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3812,8 +3959,8 @@
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
       <c r="G80" s="5"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3821,8 +3968,8 @@
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
       <c r="G81" s="7"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3830,8 +3977,8 @@
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="18"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
       <c r="G82" s="7"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3839,8 +3986,8 @@
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3857,8 +4004,8 @@
       <c r="B85" s="2"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3866,8 +4013,8 @@
       <c r="B86" s="2"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
       <c r="G86" s="7"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3875,8 +4022,8 @@
       <c r="B87" s="2"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="18"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
       <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3893,8 +4040,8 @@
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="21"/>
       <c r="G89" s="5"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3902,8 +4049,8 @@
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
       <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3911,8 +4058,8 @@
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="20"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
       <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3920,8 +4067,8 @@
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="20"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
       <c r="G92" s="5"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3938,8 +4085,8 @@
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
       <c r="G94" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3947,8 +4094,8 @@
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
       <c r="G95" s="5"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3956,104 +4103,104 @@
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
       <c r="G96" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="199">
-    <mergeCell ref="Y30:Y37"/>
-    <mergeCell ref="AC30:AD30"/>
-    <mergeCell ref="AC31:AD31"/>
-    <mergeCell ref="AC32:AD32"/>
-    <mergeCell ref="AC33:AD33"/>
-    <mergeCell ref="AC35:AD35"/>
-    <mergeCell ref="AC36:AD36"/>
-    <mergeCell ref="AC37:AD37"/>
-    <mergeCell ref="Y39:Y46"/>
-    <mergeCell ref="AC39:AD39"/>
-    <mergeCell ref="AC40:AD40"/>
-    <mergeCell ref="AC41:AD41"/>
-    <mergeCell ref="AC42:AD42"/>
-    <mergeCell ref="AC44:AD44"/>
-    <mergeCell ref="AC45:AD45"/>
-    <mergeCell ref="AC46:AD46"/>
-    <mergeCell ref="Y12:Y19"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AC13:AD13"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="Y21:Y28"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AC27:AD27"/>
-    <mergeCell ref="AC28:AD28"/>
-    <mergeCell ref="Z1:AD2"/>
-    <mergeCell ref="Y3:Y10"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="E82:F82"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="I39:I46"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
+  <mergeCells count="208">
+    <mergeCell ref="AH1:AL2"/>
+    <mergeCell ref="AG3:AG10"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AK8:AL8"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="Q30:Q37"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="U32:V32"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="U37:V37"/>
+    <mergeCell ref="Q39:Q46"/>
+    <mergeCell ref="U39:V39"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="U46:V46"/>
+    <mergeCell ref="Q12:Q19"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="Q21:Q28"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="R1:V2"/>
+    <mergeCell ref="Q3:Q10"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="I21:I28"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="I12:I19"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J1:N2"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="I30:I37"/>
+    <mergeCell ref="M37:N37"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
@@ -4078,89 +4225,98 @@
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E44:F44"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="I30:I37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="J1:N2"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="I21:I28"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="I12:I19"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="R1:V2"/>
-    <mergeCell ref="Q3:Q10"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="Q12:Q19"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="Q21:Q28"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="Q30:Q37"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="U32:V32"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="U37:V37"/>
-    <mergeCell ref="Q39:Q46"/>
-    <mergeCell ref="U39:V39"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="U41:V41"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="U46:V46"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="I39:I46"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="Z1:AD2"/>
+    <mergeCell ref="Y3:Y10"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="Y12:Y19"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AC13:AD13"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="Y21:Y28"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="AC22:AD22"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="AC26:AD26"/>
+    <mergeCell ref="AC27:AD27"/>
+    <mergeCell ref="AC28:AD28"/>
+    <mergeCell ref="Y30:Y37"/>
+    <mergeCell ref="AC30:AD30"/>
+    <mergeCell ref="AC31:AD31"/>
+    <mergeCell ref="AC32:AD32"/>
+    <mergeCell ref="AC33:AD33"/>
+    <mergeCell ref="AC35:AD35"/>
+    <mergeCell ref="AC36:AD36"/>
+    <mergeCell ref="AC37:AD37"/>
+    <mergeCell ref="Y39:Y46"/>
+    <mergeCell ref="AC39:AD39"/>
+    <mergeCell ref="AC40:AD40"/>
+    <mergeCell ref="AC41:AD41"/>
+    <mergeCell ref="AC42:AD42"/>
+    <mergeCell ref="AC44:AD44"/>
+    <mergeCell ref="AC45:AD45"/>
+    <mergeCell ref="AC46:AD46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>